<commit_message>
More work on IndVal analysis
</commit_message>
<xml_diff>
--- a/data/snag_data.xlsx
+++ b/data/snag_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopheradlam/Desktop/Davis/Research Project/Fire Mosaics/Field work/Data entered/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopheradlam/Desktop/Davis/R/GitHub Repos/Fire_mosaics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D295ABE9-C7CE-9F4E-8B9A-895F4F6FFA68}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0EA838-8D05-8741-A5ED-B6093B7F3D90}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9760" yWindow="3680" windowWidth="24440" windowHeight="12540" xr2:uid="{390B1CCC-7978-F14D-B27A-2751C2B43D86}"/>
+    <workbookView xWindow="4360" yWindow="3680" windowWidth="24440" windowHeight="12540" xr2:uid="{390B1CCC-7978-F14D-B27A-2751C2B43D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1320949E-3170-F844-AF68-7955EDB621A2}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -422,6 +422,597 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>44</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>38</v>
+      </c>
+      <c r="C9">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>42</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>43</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>44</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>46</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>41</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>47</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>51</v>
+      </c>
+      <c r="B21">
+        <v>80</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>49</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>53</v>
+      </c>
+      <c r="B23">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>52</v>
+      </c>
+      <c r="B24">
+        <v>70</v>
+      </c>
+      <c r="C24">
+        <v>40</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>40</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>60</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>59</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>27</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>55</v>
+      </c>
+      <c r="B34">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>56</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36">
+        <v>17</v>
+      </c>
+      <c r="C36">
+        <v>50</v>
+      </c>
+      <c r="D36">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>58</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>57</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>8</v>
+      </c>
+      <c r="B40">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>12</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41">
+        <v>17</v>
+      </c>
+      <c r="C41">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>33</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>34</v>
+      </c>
+      <c r="B43">
+        <v>22</v>
+      </c>
+      <c r="C43">
+        <v>33</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>15</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>10</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>32</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>36</v>
+      </c>
+      <c r="B49">
+        <v>15</v>
+      </c>
+      <c r="C49">
+        <v>30</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>